<commit_message>
Correction erreur attribution tache
</commit_message>
<xml_diff>
--- a/Répartition Taches.xlsx
+++ b/Répartition Taches.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Divers" sheetId="2" r:id="rId1"/>
@@ -1019,9 +1019,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1687,7 +1687,7 @@
         <v>80</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -1695,7 +1695,7 @@
         <v>81</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>3</v>
+        <v>52</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2035,7 +2035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>

</xml_diff>